<commit_message>
wikidata properties round 2
</commit_message>
<xml_diff>
--- a/data/properties_people.xlsx
+++ b/data/properties_people.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katie/MetadataLab/LinkedArchives/Linked_Archives_Wikibase/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1599E33-AEBC-6E4C-81D0-8525BD7C99DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC79958C-F579-8D48-8413-984FB8CC5000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="460" windowWidth="15180" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="15180" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="properties" sheetId="1" r:id="rId1"/>
@@ -2127,8 +2127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F107"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2175,7 +2175,7 @@
         <v>231</v>
       </c>
       <c r="E2" t="str">
-        <f t="shared" ref="E2:E33" si="0">_xlfn.CONCAT("'",A2,"'",":","'",D2,"'",",")</f>
+        <f>_xlfn.CONCAT("'",A2,"'",":","'",D2,"'",",")</f>
         <v>'sex or gender':'P24',</v>
       </c>
       <c r="F2" t="s">
@@ -2196,7 +2196,7 @@
         <v>83</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E2:E33" si="0">_xlfn.CONCAT("'",A3,"'",":","'",D3,"'",",")</f>
         <v>'occupation':'P25',</v>
       </c>
       <c r="F3" t="s">
@@ -4191,7 +4191,7 @@
         <v>298</v>
       </c>
       <c r="E98" t="str">
-        <f t="shared" ref="E98:E129" si="3">_xlfn.CONCAT("'",A98,"'",":","'",D98,"'",",")</f>
+        <f t="shared" ref="E98:E107" si="3">_xlfn.CONCAT("'",A98,"'",":","'",D98,"'",",")</f>
         <v>'honorific suffix':'P120',</v>
       </c>
       <c r="F98" t="s">

</xml_diff>